<commit_message>
add method details, integration period and time
- new tables OPIntegrationTimes and BLIntegrationTimes in the method struct
- updates to Excel workbook for reorganization
</commit_message>
<xml_diff>
--- a/GroundUpMCMC/GroundUpMCMC_Iteration8/DataDictionaryAndOrganization.xlsx
+++ b/GroundUpMCMC/GroundUpMCMC_Iteration8/DataDictionaryAndOrganization.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n733m382/Documents/GitHub/MCTripoli-matlab/GroundUpMCMC/GroundUpMCMC_Iteration8/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n733m382/Library/CloudStorage/Dropbox/My Mac (KU-C02DG1NKML86)/Documents/GitHub/MCTripoli-matlab/GroundUpMCMC/GroundUpMCMC_Iteration8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21408E78-CC0D-3C45-AD69-310D4A732DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD4C464-BE39-4948-B9C5-21DF2C9C1520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="43400" windowHeight="28240" activeTab="1" xr2:uid="{6405E4B5-E9F0-BB4E-B6B5-CFB878E92382}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21380" windowHeight="17500" activeTab="2" xr2:uid="{6405E4B5-E9F0-BB4E-B6B5-CFB878E92382}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="227">
   <si>
     <t>method name</t>
   </si>
@@ -714,6 +714,12 @@
   </si>
   <si>
     <t>zero</t>
+  </si>
+  <si>
+    <t>massSpec model</t>
+  </si>
+  <si>
+    <t>method struct, new tables</t>
   </si>
 </sst>
 </file>
@@ -829,13 +835,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1732,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E4B295-D6E2-B749-BEB1-3EBF113ED04F}">
   <dimension ref="A2:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1750,22 +1756,22 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="H4" s="15" t="s">
+      <c r="F4" s="16"/>
+      <c r="H4" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="14"/>
+      <c r="C5" s="15"/>
       <c r="E5" t="s">
         <v>95</v>
       </c>
@@ -2153,8 +2159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467C9259-7DF9-1B48-8017-894DE0B23E5E}">
   <dimension ref="B1:D48"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2168,7 +2174,7 @@
       <c r="B1" s="10"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2210,6 +2216,9 @@
       <c r="C9" t="s">
         <v>168</v>
       </c>
+      <c r="D9" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
@@ -2218,6 +2227,9 @@
       <c r="C10" t="s">
         <v>168</v>
       </c>
+      <c r="D10" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
@@ -2226,6 +2238,9 @@
       <c r="C11" t="s">
         <v>177</v>
       </c>
+      <c r="D11" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
@@ -2234,6 +2249,9 @@
       <c r="C12" t="s">
         <v>179</v>
       </c>
+      <c r="D12" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
@@ -2258,6 +2276,9 @@
       <c r="C17" t="s">
         <v>173</v>
       </c>
+      <c r="D17" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
@@ -2265,6 +2286,9 @@
       </c>
       <c r="C18" t="s">
         <v>187</v>
+      </c>
+      <c r="D18" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
build new class for model parameters
This class might have too many properties -- break into smaller pieces?

Update DataDictionaryAndOrganization accordingly.
</commit_message>
<xml_diff>
--- a/GroundUpMCMC/GroundUpMCMC_Iteration8/DataDictionaryAndOrganization.xlsx
+++ b/GroundUpMCMC/GroundUpMCMC_Iteration8/DataDictionaryAndOrganization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n733m382/Library/CloudStorage/Dropbox/My Mac (KU-C02DG1NKML86)/Documents/GitHub/MCTripoli-matlab/GroundUpMCMC/GroundUpMCMC_Iteration8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD4C464-BE39-4948-B9C5-21DF2C9C1520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1135A20-0031-0E4D-8A9F-2BEA3492808C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21380" windowHeight="17500" activeTab="2" xr2:uid="{6405E4B5-E9F0-BB4E-B6B5-CFB878E92382}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{6405E4B5-E9F0-BB4E-B6B5-CFB878E92382}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="231">
   <si>
     <t>method name</t>
   </si>
@@ -716,10 +716,22 @@
     <t>zero</t>
   </si>
   <si>
-    <t>massSpec model</t>
-  </si>
-  <si>
-    <t>method struct, new tables</t>
+    <t>massSpecModel property</t>
+  </si>
+  <si>
+    <t>mass property</t>
+  </si>
+  <si>
+    <t>method struct</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>OG?</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -1205,7 +1217,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1738,8 +1750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E4B295-D6E2-B749-BEB1-3EBF113ED04F}">
   <dimension ref="A2:J34"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2159,15 +2171,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467C9259-7DF9-1B48-8017-894DE0B23E5E}">
   <dimension ref="B1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
-    <col min="3" max="3" width="37.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="44.1640625" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.2">
@@ -2277,7 +2289,7 @@
         <v>173</v>
       </c>
       <c r="D17" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
@@ -2288,7 +2300,7 @@
         <v>187</v>
       </c>
       <c r="D18" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
@@ -2298,6 +2310,9 @@
       <c r="C19" t="s">
         <v>183</v>
       </c>
+      <c r="D19" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
@@ -2306,6 +2321,9 @@
       <c r="C20" t="s">
         <v>183</v>
       </c>
+      <c r="D20" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
@@ -2314,6 +2332,9 @@
       <c r="C21" s="12" t="s">
         <v>183</v>
       </c>
+      <c r="D21" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
@@ -2322,6 +2343,9 @@
       <c r="C22" t="s">
         <v>184</v>
       </c>
+      <c r="D22" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
@@ -2330,6 +2354,9 @@
       <c r="C23" t="s">
         <v>183</v>
       </c>
+      <c r="D23" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
@@ -2354,6 +2381,9 @@
       <c r="C28" t="s">
         <v>168</v>
       </c>
+      <c r="D28" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
@@ -2362,6 +2392,9 @@
       <c r="C29" t="s">
         <v>174</v>
       </c>
+      <c r="D29" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
@@ -2369,6 +2402,14 @@
       </c>
       <c r="C30" t="s">
         <v>189</v>
+      </c>
+      <c r="D30" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
@@ -2507,10 +2548,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CB0EA81-8386-0842-862A-C216DC51199B}">
-  <dimension ref="B3:L19"/>
+  <dimension ref="A3:L19"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2526,7 +2567,10 @@
     <col min="11" max="11" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>229</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>119</v>
       </c>
@@ -2561,7 +2605,10 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>230</v>
+      </c>
       <c r="B4" t="s">
         <v>121</v>
       </c>
@@ -2596,7 +2643,10 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>230</v>
+      </c>
       <c r="B5" t="s">
         <v>121</v>
       </c>
@@ -2613,7 +2663,10 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>230</v>
+      </c>
       <c r="B6" t="s">
         <v>121</v>
       </c>
@@ -2630,7 +2683,10 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>230</v>
+      </c>
       <c r="B8" t="s">
         <v>147</v>
       </c>
@@ -2653,7 +2709,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>148</v>
       </c>
@@ -2676,7 +2732,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>124</v>
       </c>
@@ -2708,7 +2764,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>125</v>
       </c>
@@ -2716,7 +2772,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>125</v>
       </c>
@@ -2724,7 +2780,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>128</v>
       </c>
@@ -2732,7 +2788,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>128</v>
       </c>
@@ -2740,7 +2796,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>131</v>
       </c>

</xml_diff>

<commit_message>
work on incorporating model parameters
</commit_message>
<xml_diff>
--- a/GroundUpMCMC/GroundUpMCMC_Iteration8/DataDictionaryAndOrganization.xlsx
+++ b/GroundUpMCMC/GroundUpMCMC_Iteration8/DataDictionaryAndOrganization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n733m382/Library/CloudStorage/Dropbox/My Mac (KU-C02DG1NKML86)/Documents/GitHub/MCTripoli-matlab/GroundUpMCMC/GroundUpMCMC_Iteration8/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n733m382/Documents/GitHub/MCTripoli-matlab/GroundUpMCMC/GroundUpMCMC_Iteration8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1135A20-0031-0E4D-8A9F-2BEA3492808C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C65794-6A64-0D4C-9417-28C9FDC91315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{6405E4B5-E9F0-BB4E-B6B5-CFB878E92382}"/>
+    <workbookView xWindow="18780" yWindow="5180" windowWidth="28800" windowHeight="22480" activeTab="1" xr2:uid="{6405E4B5-E9F0-BB4E-B6B5-CFB878E92382}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="233">
   <si>
     <t>method name</t>
   </si>
@@ -732,6 +732,12 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>non-measured species</t>
+  </si>
+  <si>
+    <t>hard-code</t>
   </si>
 </sst>
 </file>
@@ -1750,8 +1756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E4B295-D6E2-B749-BEB1-3EBF113ED04F}">
   <dimension ref="A2:J34"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2150,6 +2156,12 @@
       </c>
     </row>
     <row r="32" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>231</v>
+      </c>
+      <c r="F32" t="s">
+        <v>232</v>
+      </c>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
@@ -2550,8 +2562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CB0EA81-8386-0842-862A-C216DC51199B}">
   <dimension ref="A3:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
synthetic daat for GroundUp8a
</commit_message>
<xml_diff>
--- a/GroundUpMCMC/GroundUpMCMC_Iteration8/DataDictionaryAndOrganization.xlsx
+++ b/GroundUpMCMC/GroundUpMCMC_Iteration8/DataDictionaryAndOrganization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n733m382/Documents/GitHub/MCTripoli-matlab/GroundUpMCMC/GroundUpMCMC_Iteration8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C65794-6A64-0D4C-9417-28C9FDC91315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71E7B93-E360-DB4C-B91C-DDDFB6E278F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18780" yWindow="5180" windowWidth="28800" windowHeight="22480" activeTab="1" xr2:uid="{6405E4B5-E9F0-BB4E-B6B5-CFB878E92382}"/>
+    <workbookView xWindow="19340" yWindow="1720" windowWidth="21260" windowHeight="26840" activeTab="1" xr2:uid="{6405E4B5-E9F0-BB4E-B6B5-CFB878E92382}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -1757,7 +1757,7 @@
   <dimension ref="A2:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2133,18 +2133,18 @@
     </row>
     <row r="29" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F29" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="30" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E30" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="5:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
create and populate modelParameterSet
holds information about all unknowns needed to model system
</commit_message>
<xml_diff>
--- a/GroundUpMCMC/GroundUpMCMC_Iteration8/DataDictionaryAndOrganization.xlsx
+++ b/GroundUpMCMC/GroundUpMCMC_Iteration8/DataDictionaryAndOrganization.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n733m382/Documents/GitHub/MCTripoli-matlab/GroundUpMCMC/GroundUpMCMC_Iteration8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71E7B93-E360-DB4C-B91C-DDDFB6E278F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5D0999-1BB1-F741-AB33-B45595A24803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19340" yWindow="1720" windowWidth="21260" windowHeight="26840" activeTab="1" xr2:uid="{6405E4B5-E9F0-BB4E-B6B5-CFB878E92382}"/>
+    <workbookView xWindow="23160" yWindow="1720" windowWidth="24740" windowHeight="26840" activeTab="4" xr2:uid="{6405E4B5-E9F0-BB4E-B6B5-CFB878E92382}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
     <sheet name="unknowns" sheetId="2" r:id="rId2"/>
     <sheet name="data" sheetId="4" r:id="rId3"/>
     <sheet name="interference" sheetId="3" r:id="rId4"/>
+    <sheet name="system" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="262">
   <si>
     <t>method name</t>
   </si>
@@ -738,6 +740,93 @@
   </si>
   <si>
     <t>hard-code</t>
+  </si>
+  <si>
+    <t>for syn data</t>
+  </si>
+  <si>
+    <t>derived</t>
+  </si>
+  <si>
+    <t>config</t>
+  </si>
+  <si>
+    <t>method.massIDs</t>
+  </si>
+  <si>
+    <t>206Pb</t>
+  </si>
+  <si>
+    <t>208Pb</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>mySample.species</t>
+  </si>
+  <si>
+    <t>204Pb</t>
+  </si>
+  <si>
+    <t>207Pb</t>
+  </si>
+  <si>
+    <t>log(208/206)</t>
+  </si>
+  <si>
+    <t>isFree</t>
+  </si>
+  <si>
+    <t>Ax</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>method.OPTable</t>
+  </si>
+  <si>
+    <t>(active collectors)</t>
+  </si>
+  <si>
+    <t>1. From the user, get the path to the method file (if not found at default relative path). Parse the method (TIMSAM) file to create the method struct.</t>
+  </si>
+  <si>
+    <t>setup.methodsFolder = "./massSpecMethods/";</t>
+  </si>
+  <si>
+    <t>Outline of creating a "system" to solve, which is the same thing as creating a fully populated parameterSet object</t>
+  </si>
+  <si>
+    <t>if analyte is a referenceMaterial, then offer a constrained list of reference materials, which can be edited or appended to.  See referenceMaterial class.</t>
+  </si>
+  <si>
+    <t>If analyte is an unknown sample, then get user input for name, element (list from periodic table), species (list from isotopic table), and relativeAbundances. See sample class</t>
+  </si>
+  <si>
+    <t>2. From the user, get the analyte type. These can be associated 1:1 with the method, but can't be read directly from the method file.</t>
+  </si>
+  <si>
+    <t>3. From method, get mass IDs</t>
+  </si>
+  <si>
+    <t>4. check that these are a subset of the species field of the sample object</t>
+  </si>
+  <si>
+    <t>5. Let the user formulate (log-)ratios for the species. First, pick a common denomintor species. Then, let the user choose whether each ratio is either "free" or "assumed"</t>
+  </si>
+  <si>
+    <t>7. From the method, get the active collectors (those with an entry in the  method.OPTable)</t>
+  </si>
+  <si>
+    <t>6. From the user, get the number of spline segments and the spline degree (nSeg and bDeg). Default to bdeg = 3 and nseg = cyclesPerBlock/2</t>
+  </si>
+  <si>
+    <t>nseg</t>
+  </si>
+  <si>
+    <t>bdeg</t>
   </si>
 </sst>
 </file>
@@ -801,7 +890,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -811,6 +900,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -836,7 +931,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -858,6 +953,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1223,7 +1323,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1756,8 +1856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E4B295-D6E2-B749-BEB1-3EBF113ED04F}">
   <dimension ref="A2:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2181,10 +2281,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467C9259-7DF9-1B48-8017-894DE0B23E5E}">
-  <dimension ref="B1:D48"/>
+  <dimension ref="B1:E48"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2424,7 +2524,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>191</v>
       </c>
@@ -2432,7 +2532,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="13" t="s">
         <v>76</v>
       </c>
@@ -2442,8 +2542,11 @@
       <c r="D38" s="11" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E38" s="17" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>192</v>
       </c>
@@ -2453,8 +2556,11 @@
       <c r="D39" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E39" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>193</v>
       </c>
@@ -2464,8 +2570,11 @@
       <c r="D40" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E40" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>172</v>
       </c>
@@ -2475,8 +2584,11 @@
       <c r="D41" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E41" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>196</v>
       </c>
@@ -2486,8 +2598,11 @@
       <c r="D42" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E42" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>197</v>
       </c>
@@ -2497,8 +2612,11 @@
       <c r="D43" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E43" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>198</v>
       </c>
@@ -2508,8 +2626,11 @@
       <c r="D44" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E44" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>199</v>
       </c>
@@ -2519,8 +2640,11 @@
       <c r="D45" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E45" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>200</v>
       </c>
@@ -2530,8 +2654,11 @@
       <c r="D46" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E46" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>202</v>
       </c>
@@ -2541,8 +2668,11 @@
       <c r="D47" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E47" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>204</v>
       </c>
@@ -2551,6 +2681,9 @@
       </c>
       <c r="D48" t="s">
         <v>212</v>
+      </c>
+      <c r="E48" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -2843,4 +2976,164 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD083B2A-FEBC-3640-BEDC-F3C1020139F2}">
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="18" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="18" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="18" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>236</v>
+      </c>
+      <c r="D14" t="s">
+        <v>237</v>
+      </c>
+      <c r="E14" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>238</v>
+      </c>
+      <c r="E15" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>240</v>
+      </c>
+      <c r="D19" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D26" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D27" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="E27" s="18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D31" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D32" s="18">
+        <v>2</v>
+      </c>
+      <c r="E32" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>247</v>
+      </c>
+      <c r="D36" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>248</v>
+      </c>
+      <c r="D37" t="s">
+        <v>246</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
outlining syndata parameters and inputs
</commit_message>
<xml_diff>
--- a/GroundUpMCMC/GroundUpMCMC_Iteration8/DataDictionaryAndOrganization.xlsx
+++ b/GroundUpMCMC/GroundUpMCMC_Iteration8/DataDictionaryAndOrganization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n733m382/Documents/GitHub/MCTripoli-matlab/GroundUpMCMC/GroundUpMCMC_Iteration8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5D0999-1BB1-F741-AB33-B45595A24803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0430456-A165-C140-9112-6F3A5D150B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23160" yWindow="1720" windowWidth="24740" windowHeight="26840" activeTab="4" xr2:uid="{6405E4B5-E9F0-BB4E-B6B5-CFB878E92382}"/>
+    <workbookView xWindow="23160" yWindow="1720" windowWidth="24740" windowHeight="26840" activeTab="5" xr2:uid="{6405E4B5-E9F0-BB4E-B6B5-CFB878E92382}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="data" sheetId="4" r:id="rId3"/>
     <sheet name="interference" sheetId="3" r:id="rId4"/>
     <sheet name="system" sheetId="5" r:id="rId5"/>
+    <sheet name="syndata" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="278">
   <si>
     <t>method name</t>
   </si>
@@ -827,6 +828,54 @@
   </si>
   <si>
     <t>bdeg</t>
+  </si>
+  <si>
+    <t>8. From the mass spectrometer model, determine whether each collector is a Faraday or Ion Counter</t>
+  </si>
+  <si>
+    <t>isa(massSpec.collectorArray(["Ax"],:).collectors, "faradayModel")</t>
+  </si>
+  <si>
+    <t>isa(massSpec.collectorArray(["H1"],:).collectors, "faradayModel")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. If any Faradays: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. If any IonCounters: </t>
+  </si>
+  <si>
+    <t>enable betaFaraday, upMassTailFaraday, and downMassTailFaraday as model parameters</t>
+  </si>
+  <si>
+    <t>enable betaIonCounter, darkNoise, upMassIonCounter, and downMassIonCounter as model parameters</t>
+  </si>
+  <si>
+    <t>10. Future: add interferences</t>
+  </si>
+  <si>
+    <t>parameterization TBA</t>
+  </si>
+  <si>
+    <t>To create synthetic data, we need to combine data from the method, the mass spectrometer, and from user-specific input</t>
+  </si>
+  <si>
+    <t>To create the true modelParameters:</t>
+  </si>
+  <si>
+    <t>Initiate the system as described in the "system" sheet.</t>
+  </si>
+  <si>
+    <t>uses: method, massSpec, user input</t>
+  </si>
+  <si>
+    <t>Additional information needed to produce the data from the "data" sheet:</t>
+  </si>
+  <si>
+    <t>Intensity function (as spline knots values)</t>
+  </si>
+  <si>
+    <t>Measurement time stamps (need integration times from method for consistency)</t>
   </si>
 </sst>
 </file>
@@ -1857,7 +1906,7 @@
   <dimension ref="A2:J34"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:F12"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2283,8 +2332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467C9259-7DF9-1B48-8017-894DE0B23E5E}">
   <dimension ref="B1:E48"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2980,10 +3029,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD083B2A-FEBC-3640-BEDC-F3C1020139F2}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3112,12 +3161,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>247</v>
       </c>
@@ -3125,12 +3174,113 @@
         <v>245</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>248</v>
       </c>
       <c r="D37" t="s">
         <v>246</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>263</v>
+      </c>
+      <c r="H41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>264</v>
+      </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>270</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623F695E-F03B-9049-908F-D1C324C395C8}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tuesday morning PI meeting discussions
</commit_message>
<xml_diff>
--- a/GroundUpMCMC/GroundUpMCMC_Iteration8/DataDictionaryAndOrganization.xlsx
+++ b/GroundUpMCMC/GroundUpMCMC_Iteration8/DataDictionaryAndOrganization.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n733m382/Documents/GitHub/MCTripoli-matlab/GroundUpMCMC/GroundUpMCMC_Iteration8/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n733m382/Library/CloudStorage/Dropbox/My Mac (KU-C02DG1NKML86)/Documents/GitHub/MCTripoli-matlab/GroundUpMCMC/GroundUpMCMC_Iteration8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6059C91A-7350-0444-BE58-DA229372A46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A089ED-0C9A-A842-8AA2-221C23BADA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23160" yWindow="1720" windowWidth="24740" windowHeight="26840" activeTab="5" xr2:uid="{6405E4B5-E9F0-BB4E-B6B5-CFB878E92382}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{6405E4B5-E9F0-BB4E-B6B5-CFB878E92382}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <sheet name="syndata" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="280">
   <si>
     <t>method name</t>
   </si>
@@ -764,9 +763,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>mySample.species</t>
-  </si>
-  <si>
     <t>204Pb</t>
   </si>
   <si>
@@ -812,12 +808,6 @@
     <t>3. From method, get mass IDs</t>
   </si>
   <si>
-    <t>4. check that these are a subset of the species field of the sample object</t>
-  </si>
-  <si>
-    <t>5. Let the user formulate (log-)ratios for the species. First, pick a common denomintor species. Then, let the user choose whether each ratio is either "free" or "assumed"</t>
-  </si>
-  <si>
     <t>7. From the method, get the active collectors (those with an entry in the  method.OPTable)</t>
   </si>
   <si>
@@ -879,6 +869,18 @@
   </si>
   <si>
     <t>Measurement time stamps (derived from n, and from integration times from method for consistency)</t>
+  </si>
+  <si>
+    <t>4. check that these are a subset of the species field of the analyte object</t>
+  </si>
+  <si>
+    <t>myAnalyte.species</t>
+  </si>
+  <si>
+    <t>5. Let the user formulate (log-)ratios for the species. First, pick a common denomintor species, suggested to the user as the most abundant. Then, let the user choose whether each ratio is either "free" or "assumed"</t>
+  </si>
+  <si>
+    <t>5 revised: If all logratios are free, then user picks the denominator isotope, with a suggestion that it be the most abundant. If one or more ratios isFree=false, then the user-chosen denominator isotope must be one of the species in the chosen ratios.</t>
   </si>
 </sst>
 </file>
@@ -983,7 +985,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1001,15 +1003,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1908,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E4B295-D6E2-B749-BEB1-3EBF113ED04F}">
   <dimension ref="A2:J34"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1926,22 +1927,22 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="H4" s="16" t="s">
+      <c r="F4" s="18"/>
+      <c r="H4" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="17"/>
       <c r="E5" t="s">
         <v>95</v>
       </c>
@@ -2335,8 +2336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467C9259-7DF9-1B48-8017-894DE0B23E5E}">
   <dimension ref="B1:E48"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2594,7 +2595,7 @@
       <c r="D38" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E38" t="s">
         <v>233</v>
       </c>
     </row>
@@ -3032,47 +3033,47 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD083B2A-FEBC-3640-BEDC-F3C1020139F2}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="15" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="18" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="15" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="15" t="s">
         <v>252</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="18" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -3096,15 +3097,15 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
+        <v>277</v>
+      </c>
+      <c r="D19" t="s">
         <v>240</v>
-      </c>
-      <c r="D19" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -3114,7 +3115,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -3124,116 +3125,121 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D27" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D28" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="E28" s="15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D32" s="16" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D26" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D27" s="18" t="s">
-        <v>243</v>
-      </c>
-      <c r="E27" s="18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D31" s="19" t="s">
-        <v>260</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D32" s="18">
+      <c r="E32" s="16" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D33" s="15">
         <v>2</v>
       </c>
-      <c r="E32" s="18">
+      <c r="E33" s="15">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>247</v>
-      </c>
-      <c r="D36" t="s">
-        <v>245</v>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D37" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>263</v>
-      </c>
-      <c r="H41" t="b">
-        <v>1</v>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>247</v>
+      </c>
+      <c r="D38" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="H42" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>261</v>
+      </c>
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
         <v>267</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
-        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -3245,50 +3251,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623F695E-F03B-9049-908F-D1C324C395C8}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scott tasks for dataset class constructor
</commit_message>
<xml_diff>
--- a/GroundUpMCMC/GroundUpMCMC_Iteration8/DataDictionaryAndOrganization.xlsx
+++ b/GroundUpMCMC/GroundUpMCMC_Iteration8/DataDictionaryAndOrganization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n733m382/Library/CloudStorage/Dropbox/My Mac (KU-C02DG1NKML86)/Documents/GitHub/MCTripoli-matlab/GroundUpMCMC/GroundUpMCMC_Iteration8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A089ED-0C9A-A842-8AA2-221C23BADA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E68D51-9471-D64B-AFE5-960F272DB7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{6405E4B5-E9F0-BB4E-B6B5-CFB878E92382}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{6405E4B5-E9F0-BB4E-B6B5-CFB878E92382}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="284">
   <si>
     <t>method name</t>
   </si>
@@ -881,6 +881,18 @@
   </si>
   <si>
     <t>5 revised: If all logratios are free, then user picks the denominator isotope, with a suggestion that it be the most abundant. If one or more ratios isFree=false, then the user-chosen denominator isotope must be one of the species in the chosen ratios.</t>
+  </si>
+  <si>
+    <t>isUsed</t>
+  </si>
+  <si>
+    <t>mutable: modified by the user</t>
+  </si>
+  <si>
+    <t>all True</t>
+  </si>
+  <si>
+    <t>user sculpting</t>
   </si>
 </sst>
 </file>
@@ -1909,8 +1921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E4B295-D6E2-B749-BEB1-3EBF113ED04F}">
   <dimension ref="A2:J34"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2334,10 +2346,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467C9259-7DF9-1B48-8017-894DE0B23E5E}">
-  <dimension ref="B1:E48"/>
+  <dimension ref="B1:E49"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2737,6 +2749,20 @@
       </c>
       <c r="E48" t="s">
         <v>213</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>280</v>
+      </c>
+      <c r="C49" t="s">
+        <v>281</v>
+      </c>
+      <c r="D49" t="s">
+        <v>283</v>
+      </c>
+      <c r="E49" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -3035,8 +3061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD083B2A-FEBC-3640-BEDC-F3C1020139F2}">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>